<commit_message>
tasks file to create the task manager imports
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="161">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -145,6 +143,360 @@
   </si>
   <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t>Check all compressor status' for the LED on the main page</t>
+  </si>
+  <si>
+    <t>FaultCompressors</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Comp Rack Fault `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond Rack Fault `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond Status `%rackname` `%sgname` `%compname`</t>
+  </si>
+  <si>
+    <t>Check all condensers status' for the LED on the main page</t>
+  </si>
+  <si>
+    <t>FaultCondensers</t>
+  </si>
+  <si>
+    <t>kWh_Cond_Sum</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Calculates the running kWh total for condensers on a Rack</t>
+  </si>
+  <si>
+    <t>Cond kWh Actual `%rackname`,Cond kWh DayStart `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond kWh DayCount `%rackname`</t>
+  </si>
+  <si>
+    <t>Calculates the running kWh total for the Rack</t>
+  </si>
+  <si>
+    <t>kWh_Sum</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>kWh Actual `%rackname`,Op kWh Current Day `%rackname`,Op kWh Current Month `%rackname`,Op kWh Current Year `%rackname`,Cond kWh DayCount `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Day `%rackname`,Op kWh Counter Current Month `%rackname`,Op kWh Counter Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>Convert OP Cost kWh to OP Cost Sum</t>
+  </si>
+  <si>
+    <t>OperatingCosts</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Store $/kWh,Op kWh Counter Current Day `%rackname`,Op kWh Counter Current Month `%rackname`,Op kWh Counter Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Sum Current Day `%rackname`,Op Cost Sum Current Month `%rackname`,Op Cost Sum Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>3-59/1 * * * *</t>
+  </si>
+  <si>
+    <t>Adds the condenser and the rack predicted kw values to the Performance kW Sum variable</t>
+  </si>
+  <si>
+    <t>PredictedRackSumkW</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Performance kW Sum Predicted `%rackname`</t>
+  </si>
+  <si>
+    <t>kW Predicted `%rackname`,Cond kW Predicted `%rackname`</t>
+  </si>
+  <si>
+    <t>Calculate SEI for an individual rack</t>
+  </si>
+  <si>
+    <t>SEI_ALL_VALUES</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Refrigerant Type `%rackname`,Store Outside Temp,Cond Outlet Pressure `%rackname`,Cond Outlet Temperature `%rackname`,Discharge Pressure Actual `%rackname`,Discharge Tmp `%rackname`,Suction Temp `%rackname` `%sgname`,Suction Pressure Actual `%rackname` `%sgname`,SEI `%rackname`</t>
+  </si>
+  <si>
+    <t>COP `%rackname`,SEI `%rackname`,Liquid Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
+  </si>
+  <si>
+    <t>SetCurrentCost</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Op Cost Sum Current Day `%rackname`</t>
+  </si>
+  <si>
+    <t>Reset a time period for the Operating Cost. DAY PERIOD</t>
+  </si>
+  <si>
+    <t>Op Cost Previous Day `%rackname`,Op Cost Sum Current Day `%rackname`</t>
+  </si>
+  <si>
+    <t>2 0 * * *</t>
+  </si>
+  <si>
+    <t>Reset a time period for the kWh. DAY PERIOD</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>SetCurrentKWhMultiple</t>
+  </si>
+  <si>
+    <t>1 0 * * *</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Day `%rackname`,kWh Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Previous Day `%rackname`,Op kWh Current Day `%rackname`,Op kWh Counter Current Day `%rackname`</t>
+  </si>
+  <si>
+    <t>Reset a time period for the kWh. MONTH PERIOD</t>
+  </si>
+  <si>
+    <t>Reset a time period for the kWh. YEAR PERIOD</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Month `%rackname`,kWh Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Year `%rackname`,kWh Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Previous Month `%rackname`,Op kWh Current Month `%rackname`,Op kWh Counter Current Month `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Previous Year `%rackname`,Op kWh Current Year `%rackname`,Op kWh Counter Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>1 0 1 * *</t>
+  </si>
+  <si>
+    <t>1 0 1 1 *</t>
+  </si>
+  <si>
+    <t>Reset a time period for the Operating Cost. MONTH PERIOD</t>
+  </si>
+  <si>
+    <t>Reset a time period for the Operating Cost. YEAR PERIOD</t>
+  </si>
+  <si>
+    <t>Op Cost Sum Current Month `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Previous Month `%rackname`,Op Cost Sum Current Month `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Sum Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Previous Year `%rackname`,Op Cost Sum Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>2 0 1 * *</t>
+  </si>
+  <si>
+    <t>2 0 1 1 *</t>
+  </si>
+  <si>
+    <t>Calculate the store costs for the financial page.</t>
+  </si>
+  <si>
+    <t>StoreCosts</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Energy COP Avg,Store $/kWh,Op Cost Total Previous Month,Store Sqft</t>
+  </si>
+  <si>
+    <t>Energy KBTU/kW Capacity,Energy MBTU/hour Cost,Energy Cost/SqFt</t>
+  </si>
+  <si>
+    <t>Cond kWh DayStart `%rackname`,Cond kWh DayCount `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond kWh Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>SetCurrentkWhCondMultiple</t>
+  </si>
+  <si>
+    <t>Reset the Cond kWh counter at 12:01am</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Performance kW Sum Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>kW Actual `%rackname`,Cond kW Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>Adds the item up. Performance kW Sum</t>
+  </si>
+  <si>
+    <t>Performance Total kW Sum Actual</t>
+  </si>
+  <si>
+    <t>Performance Cost Sum Actual `%rackname`</t>
+  </si>
+  <si>
+    <t>Performance Total Cost Sum Actual</t>
+  </si>
+  <si>
+    <t>Adds the item up. Performance Total Cost</t>
+  </si>
+  <si>
+    <t>Op kWh Total Previous Day</t>
+  </si>
+  <si>
+    <t>Op kWh Previous Day `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Previous Month `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Total Previous Month</t>
+  </si>
+  <si>
+    <t>Op kWh Previous Year `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Total Previous Year</t>
+  </si>
+  <si>
+    <t>Op Cost Previous Day `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Previous Month `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Previous Year `%rackname`</t>
+  </si>
+  <si>
+    <t>Op Cost Total Sum Current Day</t>
+  </si>
+  <si>
+    <t>Op Cost Total Sum Current Month</t>
+  </si>
+  <si>
+    <t>Op Cost Total Sum Current Year</t>
+  </si>
+  <si>
+    <t>Operating Cost Current Day</t>
+  </si>
+  <si>
+    <t>Operating Cost Current Month</t>
+  </si>
+  <si>
+    <t>Operating Cost Current Year</t>
+  </si>
+  <si>
+    <t>Operating Cost Previous Day</t>
+  </si>
+  <si>
+    <t>Op Cost Total Sum Previous Day</t>
+  </si>
+  <si>
+    <t>Operating Cost Previous Month</t>
+  </si>
+  <si>
+    <t>Op Cost Total Sum Previous Month</t>
+  </si>
+  <si>
+    <t>Operating Cost Previous Year</t>
+  </si>
+  <si>
+    <t>Op Cost Total Sum Previous Year</t>
+  </si>
+  <si>
+    <t>*/5 * * * *</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Day `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Total Counter Current Day</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Month `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Total Counter Current Month</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Year `%rackname`</t>
+  </si>
+  <si>
+    <t>Op kWh Total Counter Current Year</t>
+  </si>
+  <si>
+    <t>Operating kWh Total Previous Day</t>
+  </si>
+  <si>
+    <t>Operating kWh Total Previous Month</t>
+  </si>
+  <si>
+    <t>Operating kWh Total Previous Year</t>
+  </si>
+  <si>
+    <t>Operating kWh Total Counter Current Day</t>
+  </si>
+  <si>
+    <t>Operating kWh Total Counter Current Month</t>
+  </si>
+  <si>
+    <t>Operating kWh Total Counter Current Year</t>
+  </si>
+  <si>
+    <t>Performance Total kW Sum Predicted</t>
+  </si>
+  <si>
+    <t>Adds the item up. Performance Total kW Sum</t>
   </si>
 </sst>
 </file>
@@ -180,9 +532,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -199,7 +550,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,241 +853,1035 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="38.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="38.140625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="38.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>24</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -744,28 +1889,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
working on task manager db imports
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="taskSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -532,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -541,16 +541,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,23 +853,23 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="38.140625" style="6" customWidth="1"/>
+    <col min="4" max="5" width="38.140625" style="4" customWidth="1"/>
     <col min="6" max="7" width="38.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -898,7 +895,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -907,10 +904,10 @@
       <c r="C2" s="1">
         <v>24</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -924,7 +921,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -933,10 +930,10 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -950,7 +947,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -959,10 +956,10 @@
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -976,7 +973,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -985,10 +982,10 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1002,7 +999,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1011,10 +1008,10 @@
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1028,7 +1025,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1037,10 +1034,10 @@
       <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1054,7 +1051,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1063,10 +1060,10 @@
       <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1080,7 +1077,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1089,10 +1086,10 @@
       <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1106,7 +1103,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1115,10 +1112,10 @@
       <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1132,7 +1129,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1141,10 +1138,10 @@
       <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1158,7 +1155,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1167,10 +1164,10 @@
       <c r="C12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1184,7 +1181,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1193,10 +1190,10 @@
       <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1210,7 +1207,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1219,10 +1216,10 @@
       <c r="C14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1236,7 +1233,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1245,10 +1242,10 @@
       <c r="C15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1262,7 +1259,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1271,10 +1268,10 @@
       <c r="C16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1287,8 +1284,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1297,10 +1294,10 @@
       <c r="C17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1314,7 +1311,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1323,10 +1320,10 @@
       <c r="C18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>95</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1340,7 +1337,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1349,10 +1346,10 @@
       <c r="C19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>82</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1366,7 +1363,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1375,10 +1372,10 @@
       <c r="C20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1392,7 +1389,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1401,10 +1398,10 @@
       <c r="C21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1418,7 +1415,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1427,10 +1424,10 @@
       <c r="C22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -1444,7 +1441,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1453,10 +1450,10 @@
       <c r="C23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1470,7 +1467,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1479,10 +1476,10 @@
       <c r="C24" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -1496,7 +1493,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>160</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1505,10 +1502,10 @@
       <c r="C25" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>121</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1522,7 +1519,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>160</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1531,10 +1528,10 @@
       <c r="C26" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>159</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1548,7 +1545,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1557,10 +1554,10 @@
       <c r="C27" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -1574,7 +1571,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
         <v>153</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1583,10 +1580,10 @@
       <c r="C28" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>125</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1600,7 +1597,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>154</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1609,10 +1606,10 @@
       <c r="C29" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>128</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1626,7 +1623,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="5" t="s">
         <v>155</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1635,10 +1632,10 @@
       <c r="C30" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>130</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -1652,7 +1649,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="5" t="s">
         <v>156</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1661,10 +1658,10 @@
       <c r="C31" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>148</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1678,7 +1675,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="5" t="s">
         <v>157</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1687,10 +1684,10 @@
       <c r="C32" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="4" t="s">
         <v>150</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -1704,7 +1701,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>158</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1713,10 +1710,10 @@
       <c r="C33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="4" t="s">
         <v>152</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -1730,7 +1727,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="5" t="s">
         <v>137</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1739,10 +1736,10 @@
       <c r="C34" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>134</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -1756,7 +1753,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="5" t="s">
         <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1765,10 +1762,10 @@
       <c r="C35" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="4" t="s">
         <v>135</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -1782,7 +1779,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>139</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1791,10 +1788,10 @@
       <c r="C36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -1808,7 +1805,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="5" t="s">
         <v>140</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1817,10 +1814,10 @@
       <c r="C37" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="4" t="s">
         <v>141</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -1834,7 +1831,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="5" t="s">
         <v>142</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1843,10 +1840,10 @@
       <c r="C38" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="4" t="s">
         <v>143</v>
       </c>
       <c r="F38" s="1" t="s">
@@ -1860,7 +1857,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="5" t="s">
         <v>144</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1869,10 +1866,10 @@
       <c r="C39" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F39" s="1" t="s">

</xml_diff>

<commit_message>
Task manager exports nearly done just need to add some db commands
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="163">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -418,15 +418,6 @@
     <t>Op Cost Previous Year `%rackname`</t>
   </si>
   <si>
-    <t>Op Cost Total Sum Current Day</t>
-  </si>
-  <si>
-    <t>Op Cost Total Sum Current Month</t>
-  </si>
-  <si>
-    <t>Op Cost Total Sum Current Year</t>
-  </si>
-  <si>
     <t>Operating Cost Current Day</t>
   </si>
   <si>
@@ -439,42 +430,24 @@
     <t>Operating Cost Previous Day</t>
   </si>
   <si>
-    <t>Op Cost Total Sum Previous Day</t>
-  </si>
-  <si>
     <t>Operating Cost Previous Month</t>
   </si>
   <si>
-    <t>Op Cost Total Sum Previous Month</t>
-  </si>
-  <si>
     <t>Operating Cost Previous Year</t>
   </si>
   <si>
-    <t>Op Cost Total Sum Previous Year</t>
-  </si>
-  <si>
     <t>*/5 * * * *</t>
   </si>
   <si>
     <t>Op kWh Counter Current Day `%rackname`</t>
   </si>
   <si>
-    <t>Op kWh Total Counter Current Day</t>
-  </si>
-  <si>
     <t>Op kWh Counter Current Month `%rackname`</t>
   </si>
   <si>
-    <t>Op kWh Total Counter Current Month</t>
-  </si>
-  <si>
     <t>Op kWh Counter Current Year `%rackname`</t>
   </si>
   <si>
-    <t>Op kWh Total Counter Current Year</t>
-  </si>
-  <si>
     <t>Operating kWh Total Previous Day</t>
   </si>
   <si>
@@ -497,6 +470,39 @@
   </si>
   <si>
     <t>Adds the item up. Performance Total kW Sum</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Op Cost Total Current Day</t>
+  </si>
+  <si>
+    <t>Op Cost Total Current Month</t>
+  </si>
+  <si>
+    <t>Op Cost Total Current Year</t>
+  </si>
+  <si>
+    <t>Op Cost Total Previous Day</t>
+  </si>
+  <si>
+    <t>Op Cost Total Previous Month</t>
+  </si>
+  <si>
+    <t>Op Cost Total Previous Year</t>
+  </si>
+  <si>
+    <t>Op kWh Total Current Day</t>
+  </si>
+  <si>
+    <t>Op kWh Total Current Month</t>
+  </si>
+  <si>
+    <t>Op kWh Total Current Year</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -854,7 +860,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +871,7 @@
     <col min="4" max="5" width="38.140625" style="4" customWidth="1"/>
     <col min="6" max="7" width="38.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -901,8 +907,8 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
-        <v>24</v>
+      <c r="C2" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -995,7 +1001,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1021,7 +1027,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1494,7 +1500,7 @@
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>116</v>
@@ -1520,7 +1526,7 @@
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>116</v>
@@ -1532,7 +1538,7 @@
         <v>71</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>10</v>
@@ -1572,7 +1578,7 @@
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>116</v>
@@ -1598,7 +1604,7 @@
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>116</v>
@@ -1624,7 +1630,7 @@
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>116</v>
@@ -1650,7 +1656,7 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>116</v>
@@ -1659,10 +1665,10 @@
         <v>117</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>10</v>
@@ -1676,7 +1682,7 @@
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>116</v>
@@ -1685,10 +1691,10 @@
         <v>117</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>10</v>
@@ -1702,7 +1708,7 @@
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>116</v>
@@ -1711,10 +1717,10 @@
         <v>117</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>10</v>
@@ -1728,7 +1734,7 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>116</v>
@@ -1740,7 +1746,7 @@
         <v>80</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>10</v>
@@ -1754,7 +1760,7 @@
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>116</v>
@@ -1766,7 +1772,7 @@
         <v>100</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>10</v>
@@ -1780,7 +1786,7 @@
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>116</v>
@@ -1792,7 +1798,7 @@
         <v>102</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>10</v>
@@ -1806,7 +1812,7 @@
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>116</v>
@@ -1818,10 +1824,10 @@
         <v>131</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
@@ -1832,7 +1838,7 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>116</v>
@@ -1844,10 +1850,10 @@
         <v>132</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
@@ -1858,7 +1864,7 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>116</v>
@@ -1870,10 +1876,10 @@
         <v>133</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updated postgres jar. Fixed task manager task generation. Import to database working.
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="8805" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="taskSheet" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="178">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -37,9 +37,6 @@
     <t>EachRack</t>
   </si>
   <si>
-    <t>Actual_Costs_kW</t>
-  </si>
-  <si>
     <t>Store $/kWh,Performance kW Sum Predicted `%rackname`,Performance kW Sum Actual `%rackname`,Performance kW Sum Difference `%rackname`</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>Average all Rack SEI values into a total variable</t>
   </si>
   <si>
-    <t>Avg_Items</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>Find the compressor status for the individual compressors on the Rack</t>
   </si>
   <si>
-    <t>CompStatus</t>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>Find the condenser fan status for the individual condensers on the Rack</t>
   </si>
   <si>
-    <t>CondFanStatus</t>
-  </si>
-  <si>
     <t>Cond Fan Status `%rackname` `%fannum`</t>
   </si>
   <si>
@@ -121,18 +109,12 @@
     <t>Find the predicted value for the IO input</t>
   </si>
   <si>
-    <t>DbFindPredicted</t>
-  </si>
-  <si>
     <t>38</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>DbSavePredicted</t>
-  </si>
-  <si>
     <t>Save the demand value</t>
   </si>
   <si>
@@ -148,9 +130,6 @@
     <t>Check all compressor status' for the LED on the main page</t>
   </si>
   <si>
-    <t>FaultCompressors</t>
-  </si>
-  <si>
     <t>41</t>
   </si>
   <si>
@@ -163,18 +142,9 @@
     <t>Cond Rack Fault `%rackname`</t>
   </si>
   <si>
-    <t>Cond Status `%rackname` `%sgname` `%compname`</t>
-  </si>
-  <si>
     <t>Check all condensers status' for the LED on the main page</t>
   </si>
   <si>
-    <t>FaultCondensers</t>
-  </si>
-  <si>
-    <t>kWh_Cond_Sum</t>
-  </si>
-  <si>
     <t>26</t>
   </si>
   <si>
@@ -190,9 +160,6 @@
     <t>Calculates the running kWh total for the Rack</t>
   </si>
   <si>
-    <t>kWh_Sum</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -205,9 +172,6 @@
     <t>Convert OP Cost kWh to OP Cost Sum</t>
   </si>
   <si>
-    <t>OperatingCosts</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -223,9 +187,6 @@
     <t>Adds the condenser and the rack predicted kw values to the Performance kW Sum variable</t>
   </si>
   <si>
-    <t>PredictedRackSumkW</t>
-  </si>
-  <si>
     <t>39</t>
   </si>
   <si>
@@ -238,9 +199,6 @@
     <t>Calculate SEI for an individual rack</t>
   </si>
   <si>
-    <t>SEI_ALL_VALUES</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
@@ -250,9 +208,6 @@
     <t>COP `%rackname`,SEI `%rackname`,Liquid Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
   </si>
   <si>
-    <t>SetCurrentCost</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -274,9 +229,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>SetCurrentKWhMultiple</t>
-  </si>
-  <si>
     <t>1 0 * * *</t>
   </si>
   <si>
@@ -337,9 +289,6 @@
     <t>Calculate the store costs for the financial page.</t>
   </si>
   <si>
-    <t>StoreCosts</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
@@ -358,15 +307,9 @@
     <t>27</t>
   </si>
   <si>
-    <t>SetCurrentkWhCondMultiple</t>
-  </si>
-  <si>
     <t>Reset the Cond kWh counter at 12:01am</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
@@ -503,6 +446,108 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Avg_Items All Racks</t>
+  </si>
+  <si>
+    <t>Actual_Costs_kW All Racks</t>
+  </si>
+  <si>
+    <t>CompStatus `%rackname`</t>
+  </si>
+  <si>
+    <t>CondFanStatus `%rackname`</t>
+  </si>
+  <si>
+    <t>DbFindPredicted All Racks</t>
+  </si>
+  <si>
+    <t>DbSavePredicted All Racks</t>
+  </si>
+  <si>
+    <t>FaultCompressors All Racks</t>
+  </si>
+  <si>
+    <t>FaultCondensers All Racks</t>
+  </si>
+  <si>
+    <t>kWh_Cond_Sum All Racks</t>
+  </si>
+  <si>
+    <t>kWh_Sum All Racks</t>
+  </si>
+  <si>
+    <t>OperatingCosts All Racks</t>
+  </si>
+  <si>
+    <t>PredictedRackSumkW All Racks</t>
+  </si>
+  <si>
+    <t>SetCurrentKWhMultiple All Racks</t>
+  </si>
+  <si>
+    <t>SetCurrentCost All Racks</t>
+  </si>
+  <si>
+    <t>StoreCosts All Racks</t>
+  </si>
+  <si>
+    <t>SetCurrentkWhCondMultiple All Racks</t>
+  </si>
+  <si>
+    <t>Cond Fan Status `%rackname` `%sgname` `%compname`</t>
+  </si>
+  <si>
+    <t>SEI_ALL_VALUES `%rackname`</t>
+  </si>
+  <si>
+    <t>Sum kW `%rackname`</t>
+  </si>
+  <si>
+    <t>Sum kW Total Predicted</t>
+  </si>
+  <si>
+    <t>Sum kW Total Actual</t>
+  </si>
+  <si>
+    <t>Sum Cost Total Actual</t>
+  </si>
+  <si>
+    <t>Sum kWh Total Prev Day</t>
+  </si>
+  <si>
+    <t>Sum kWh Total Prev Month</t>
+  </si>
+  <si>
+    <t>Sum kWh Total Prev Year</t>
+  </si>
+  <si>
+    <t>Sum kWh Total Curr Day</t>
+  </si>
+  <si>
+    <t>Sum kWh Total Curr Month</t>
+  </si>
+  <si>
+    <t>Sum kWh Total Curr Year</t>
+  </si>
+  <si>
+    <t>Sum Op Cost Prev Day</t>
+  </si>
+  <si>
+    <t>Sum Op Cost Curr Year</t>
+  </si>
+  <si>
+    <t>Sum Op Cost Curr Day</t>
+  </si>
+  <si>
+    <t>Sum Op Cost Curr Month</t>
+  </si>
+  <si>
+    <t>Sum Op Cost Prev Month</t>
+  </si>
+  <si>
+    <t>Sum Op Cost Prev Year</t>
   </si>
 </sst>
 </file>
@@ -859,16 +904,17 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="38.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" style="4" customWidth="1"/>
     <col min="6" max="7" width="38.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -876,7 +922,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -902,623 +948,623 @@
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>69</v>
+        <v>155</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>11</v>
@@ -1526,25 +1572,25 @@
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>11</v>
@@ -1552,25 +1598,25 @@
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>11</v>
@@ -1578,314 +1624,314 @@
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>116</v>
+        <v>166</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>116</v>
+        <v>170</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="F35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some default io variables & default widgets. Default widgets added to jar directory. If they dont exist in the home directory, it will use the one in the jar
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="180" windowWidth="8805" windowHeight="6555"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>34</t>
   </si>
   <si>
-    <t>Comp Amps `%rackname` `%sgname` `%compname`,Comp RUN `%rackname` `%sgname` `%compname`,Comp Status `%rackname` `%sgname` `%compname`</t>
-  </si>
-  <si>
     <t>Comp Status `%rackname` `%sgname` `%compname`</t>
   </si>
   <si>
@@ -548,6 +545,9 @@
   </si>
   <si>
     <t>Sum Op Cost Prev Year</t>
+  </si>
+  <si>
+    <t>Comp Amps `%rackname` `%sgname` `%compname`,Comp SLA `%rackname` `%sgname` `%compname`,Comp Discharge Temp `%rackname` `%sgname` `%compname`</t>
   </si>
 </sst>
 </file>
@@ -901,11 +901,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,10 +952,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
@@ -977,7 +978,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -1003,7 +1004,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -1024,22 +1025,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1047,24 +1048,24 @@
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -1073,27 +1074,27 @@
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>11</v>
@@ -1104,22 +1105,22 @@
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -1130,19 +1131,19 @@
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -1156,19 +1157,19 @@
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -1182,19 +1183,19 @@
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
@@ -1208,19 +1209,19 @@
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -1234,22 +1235,22 @@
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
@@ -1260,19 +1261,19 @@
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1286,19 +1287,19 @@
     </row>
     <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1312,22 +1313,22 @@
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>10</v>
@@ -1338,22 +1339,22 @@
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>10</v>
@@ -1364,22 +1365,22 @@
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>10</v>
@@ -1390,22 +1391,22 @@
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>10</v>
@@ -1416,22 +1417,22 @@
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>10</v>
@@ -1442,22 +1443,22 @@
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>10</v>
@@ -1468,19 +1469,19 @@
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -1494,22 +1495,22 @@
     </row>
     <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>10</v>
@@ -1520,19 +1521,19 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>9</v>
@@ -1546,19 +1547,19 @@
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>9</v>
@@ -1572,19 +1573,19 @@
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>9</v>
@@ -1598,19 +1599,19 @@
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>9</v>
@@ -1624,19 +1625,19 @@
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>9</v>
@@ -1650,19 +1651,19 @@
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>9</v>
@@ -1676,19 +1677,19 @@
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
@@ -1702,19 +1703,19 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
@@ -1728,19 +1729,19 @@
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>9</v>
@@ -1754,19 +1755,19 @@
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>9</v>
@@ -1780,19 +1781,19 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>9</v>
@@ -1806,19 +1807,19 @@
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>9</v>
@@ -1832,19 +1833,19 @@
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>9</v>
@@ -1858,22 +1859,22 @@
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>10</v>
@@ -1884,22 +1885,22 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>10</v>
@@ -1910,22 +1911,22 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Glycol + Energy Pages - Not done yet
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -37,12 +37,6 @@
     <t>EachRack</t>
   </si>
   <si>
-    <t>Store $/kWh,Performance kW Sum Predicted `%rackname`,Performance kW Sum Actual `%rackname`,Performance kW Sum Difference `%rackname`</t>
-  </si>
-  <si>
-    <t>Performance Cost Sum Predicted `%rackname`,Performance Cost Sum Actual `%rackname`,Performance Cost Sum Difference `%rackname`</t>
-  </si>
-  <si>
     <t>* * * * *</t>
   </si>
   <si>
@@ -548,6 +542,12 @@
   </si>
   <si>
     <t>Comp Amps `%rackname` `%sgname` `%compname`,Comp SLA `%rackname` `%sgname` `%compname`,Comp Discharge Temp `%rackname` `%sgname` `%compname`</t>
+  </si>
+  <si>
+    <t>Store $/kWh,Performance kW Sum Predicted `%rackname`,Performance kW Sum Actual `%rackname`,Performance Total kW Sum Predicted</t>
+  </si>
+  <si>
+    <t>Performance Cost Sum Predicted `%rackname`,Performance Cost Sum Actual `%rackname`,Performance Total Cost Sum Predicted</t>
   </si>
 </sst>
 </file>
@@ -906,7 +906,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +923,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -947,992 +947,992 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="F14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="E24" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished rest of widgets on rack panel + modals on all pages
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="183">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -58,9 +58,6 @@
     <t>30</t>
   </si>
   <si>
-    <t>SEI `%rackname`</t>
-  </si>
-  <si>
     <t>Energy SEI Avg</t>
   </si>
   <si>
@@ -193,12 +190,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>Refrigerant Type `%rackname`,Store Outside Temp,Cond Outlet Pressure `%rackname`,Cond Outlet Temperature `%rackname`,Discharge Pressure Actual `%rackname`,Discharge Tmp `%rackname`,Suction Temp `%rackname` `%sgname`,Suction Pressure Actual `%rackname` `%sgname`,SEI `%rackname`</t>
-  </si>
-  <si>
-    <t>COP `%rackname`,SEI `%rackname`,Liquid Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -457,12 +448,6 @@
     <t>DbSavePredicted All Racks</t>
   </si>
   <si>
-    <t>FaultCompressors All Racks</t>
-  </si>
-  <si>
-    <t>FaultCondensers All Racks</t>
-  </si>
-  <si>
     <t>kWh_Cond_Sum All Racks</t>
   </si>
   <si>
@@ -475,12 +460,6 @@
     <t>PredictedRackSumkW All Racks</t>
   </si>
   <si>
-    <t>SetCurrentKWhMultiple All Racks</t>
-  </si>
-  <si>
-    <t>SetCurrentCost All Racks</t>
-  </si>
-  <si>
     <t>StoreCosts All Racks</t>
   </si>
   <si>
@@ -548,6 +527,42 @@
   </si>
   <si>
     <t>Performance Cost Sum Predicted `%rackname`,Performance Cost Sum Actual `%rackname`,Performance Total Cost Sum Predicted</t>
+  </si>
+  <si>
+    <t>kWh Reset Year All Racks</t>
+  </si>
+  <si>
+    <t>kWh Reset Day All Racks</t>
+  </si>
+  <si>
+    <t>kWh Reset Month All Racks</t>
+  </si>
+  <si>
+    <t>FaultCompressors `%rackname`</t>
+  </si>
+  <si>
+    <t>FaultCondensers `%rackname`</t>
+  </si>
+  <si>
+    <t>OP Cost Day</t>
+  </si>
+  <si>
+    <t>OP Cost Month</t>
+  </si>
+  <si>
+    <t>OP Cost Year</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Rack SEI `%rackname`</t>
+  </si>
+  <si>
+    <t>Refrigerant Type `%rackname`,Store Outside Temp,Cond Outlet Pressure `%rackname`,Cond Outlet Temperature `%rackname`,Discharge Pressure Actual `%rackname`,Discharge Tmp `%rackname`,Suction Temp `%rackname` `%sgname`,Suction Pressure Actual `%rackname` `%sgname`,Rack SEI `%rackname`</t>
+  </si>
+  <si>
+    <t>COP `%rackname`,Rack SEI `%rackname`,Cond Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
   </si>
 </sst>
 </file>
@@ -905,14 +920,14 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="38.140625" style="4" customWidth="1"/>
@@ -952,16 +967,16 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -978,16 +993,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -1001,19 +1016,19 @@
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -1027,20 +1042,20 @@
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1048,25 +1063,25 @@
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1074,27 +1089,27 @@
         <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
@@ -1105,22 +1120,22 @@
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>9</v>
@@ -1131,19 +1146,19 @@
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
@@ -1152,24 +1167,24 @@
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>7</v>
@@ -1178,24 +1193,24 @@
         <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -1209,19 +1224,19 @@
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>7</v>
@@ -1235,22 +1250,22 @@
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>8</v>
@@ -1261,19 +1276,19 @@
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>7</v>
@@ -1287,19 +1302,19 @@
     </row>
     <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -1308,27 +1323,27 @@
         <v>8</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>8</v>
@@ -1339,22 +1354,22 @@
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>8</v>
@@ -1365,22 +1380,22 @@
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>8</v>
@@ -1391,22 +1406,22 @@
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="F19" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>8</v>
@@ -1417,22 +1432,22 @@
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>8</v>
@@ -1443,22 +1458,22 @@
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>8</v>
@@ -1469,20 +1484,20 @@
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="F22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1490,27 +1505,27 @@
         <v>8</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>8</v>
@@ -1521,19 +1536,19 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
@@ -1547,19 +1562,19 @@
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>7</v>
@@ -1573,19 +1588,19 @@
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>7</v>
@@ -1599,19 +1614,19 @@
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>7</v>
@@ -1625,19 +1640,19 @@
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>7</v>
@@ -1651,19 +1666,19 @@
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>7</v>
@@ -1677,19 +1692,19 @@
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>7</v>
@@ -1703,19 +1718,19 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>7</v>
@@ -1729,19 +1744,19 @@
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>7</v>
@@ -1755,19 +1770,19 @@
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>7</v>
@@ -1781,19 +1796,19 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>7</v>
@@ -1807,19 +1822,19 @@
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>7</v>
@@ -1833,19 +1848,19 @@
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>7</v>
@@ -1859,22 +1874,22 @@
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>8</v>
@@ -1885,22 +1900,22 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>8</v>
@@ -1911,22 +1926,22 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated some excel and text files
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="191">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -563,6 +563,30 @@
   </si>
   <si>
     <t>COP `%rackname`,Rack SEI `%rackname`,Cond Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
+  </si>
+  <si>
+    <t>Finds the difference between the cond variables</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Cond Ambient Subcooling Difference</t>
+  </si>
+  <si>
+    <t>Cond Temp Difference</t>
+  </si>
+  <si>
+    <t>Cond Air TD `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond Outlet Air Temperature `%rackname`,Cond Inlet Air Temperature `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond Downleg Temperature `%rackname`,Cond Inlet Air Temperature `%rackname`</t>
+  </si>
+  <si>
+    <t>Cond Ambient Subcooling `%rackname`</t>
   </si>
 </sst>
 </file>
@@ -917,11 +941,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,6 +1974,58 @@
         <v>9</v>
       </c>
     </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
IO changes, task update
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -559,9 +559,6 @@
     <t>Rack SEI `%rackname`</t>
   </si>
   <si>
-    <t>Refrigerant Type `%rackname`,Store Outside Temp,Cond Outlet Pressure `%rackname`,Cond Outlet Temperature `%rackname`,Discharge Pressure Actual `%rackname`,Discharge Tmp `%rackname`,Suction Temp `%rackname` `%sgname`,Suction Pressure Actual `%rackname` `%sgname`,Rack SEI `%rackname`</t>
-  </si>
-  <si>
     <t>COP `%rackname`,Rack SEI `%rackname`,Cond Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
   </si>
   <si>
@@ -587,6 +584,9 @@
   </si>
   <si>
     <t>Cond Ambient Subcooling `%rackname`</t>
+  </si>
+  <si>
+    <t>Refrigerant Type `%rackname`,Store Outside Temp,Cond Outlet Pressure `%rackname`,Cond Outlet Air Temperature `%rackname`,Discharge Pressure Actual `%rackname`,Discharge Tmp `%rackname`,Suction Temp `%rackname` `%sgname`,Suction Pressure Actual `%rackname` `%sgname`,Rack SEI `%rackname`</t>
   </si>
 </sst>
 </file>
@@ -944,8 +944,8 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,10 +1335,10 @@
         <v>57</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -1976,19 +1976,19 @@
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>7</v>
@@ -2002,19 +2002,19 @@
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="D41" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>190</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Bug fixes, a lot of changes to add fan panels, pump skid to modbus/name generators
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -502,12 +502,6 @@
     <t>Comp Amps `%rackname` `%sgname` `%compname`,Comp SLA `%rackname` `%sgname` `%compname`,Comp Discharge Temp `%rackname` `%sgname` `%compname`</t>
   </si>
   <si>
-    <t>Store $/kWh,Performance kW Sum Predicted `%rackname`,Performance kW Sum Actual `%rackname`,Performance Total kW Sum Predicted</t>
-  </si>
-  <si>
-    <t>Performance Cost Sum Predicted `%rackname`,Performance Cost Sum Actual `%rackname`,Performance Total Cost Sum Predicted</t>
-  </si>
-  <si>
     <t>FaultCompressors `%rackname`</t>
   </si>
   <si>
@@ -599,6 +593,12 @@
   </si>
   <si>
     <t>Cond kWh YearStart `%rackname`,Cond kWh YearCount `%rackname`</t>
+  </si>
+  <si>
+    <t>Store $/kWh,Performance kW Sum Predicted `%rackname`,Performance kW Sum Actual `%rackname`,Performance Total kW Sum Predicted,Performance Total kW Sum Actual</t>
+  </si>
+  <si>
+    <t>Performance Cost Sum Predicted `%rackname`,Performance Cost Sum Actual `%rackname`,Performance Total Cost Sum Predicted,Performance Total Cost Sum Actual</t>
   </si>
 </sst>
 </file>
@@ -957,7 +957,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1009,10 +1009,10 @@
         <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -1035,7 +1035,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -1110,7 +1110,7 @@
         <v>138</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
@@ -1185,7 +1185,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
@@ -1211,7 +1211,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1237,16 +1237,16 @@
         <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -1263,13 +1263,13 @@
         <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>43</v>
@@ -1315,7 +1315,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>50</v>
@@ -1347,10 +1347,10 @@
         <v>54</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -1367,7 +1367,7 @@
         <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>61</v>
@@ -1393,7 +1393,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>61</v>
@@ -1419,7 +1419,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>61</v>
@@ -1445,7 +1445,7 @@
         <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>55</v>
@@ -1471,7 +1471,7 @@
         <v>73</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
@@ -1497,7 +1497,7 @@
         <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>55</v>
@@ -1549,7 +1549,7 @@
         <v>88</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>87</v>
@@ -1575,7 +1575,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>87</v>
@@ -1584,7 +1584,7 @@
         <v>86</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>71</v>
@@ -1601,7 +1601,7 @@
         <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>87</v>
@@ -1610,7 +1610,7 @@
         <v>86</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>72</v>
@@ -2040,19 +2040,19 @@
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="E42" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>7</v>
@@ -2066,19 +2066,19 @@
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Some updates to tasks, final bug fixes to include the new strings for glycol systems and fan panels
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="207">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -106,12 +106,6 @@
     <t>Save the demand value</t>
   </si>
   <si>
-    <t>Store Outside Temp,Cond kW Avg Demand `%rackname`,kW Avg Demand `%rackname`</t>
-  </si>
-  <si>
-    <t>Cond kW Predicted `%rackname`,kW Predicted `%rackname`</t>
-  </si>
-  <si>
     <t>Blank</t>
   </si>
   <si>
@@ -355,15 +349,6 @@
     <t>*/5 * * * *</t>
   </si>
   <si>
-    <t>Op kWh Counter Current Day `%rackname`</t>
-  </si>
-  <si>
-    <t>Op kWh Counter Current Month `%rackname`</t>
-  </si>
-  <si>
-    <t>Op kWh Counter Current Year `%rackname`</t>
-  </si>
-  <si>
     <t>Operating kWh Total Previous Day</t>
   </si>
   <si>
@@ -421,12 +406,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>Avg_Items All Racks</t>
-  </si>
-  <si>
-    <t>Actual_Costs_kW All Racks</t>
-  </si>
-  <si>
     <t>CompStatus `%rackname`</t>
   </si>
   <si>
@@ -599,6 +578,63 @@
   </si>
   <si>
     <t>Performance Cost Sum Predicted `%rackname`,Performance Cost Sum Actual `%rackname`,Performance Total Cost Sum Predicted,Performance Total Cost Sum Actual</t>
+  </si>
+  <si>
+    <t>Performance kW Sum Actual `%rackname`,Glycol Pump Skid kW Actual,Fan Panel kW Actual `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Calculates the running kWh total for other items</t>
+  </si>
+  <si>
+    <t>Glycol Pump Skid kWh DayCount,Glycol Pump Skid kWh MonthCount,Glycol Pump Skid kWh YearCount</t>
+  </si>
+  <si>
+    <t>Glycol Pump Skid kWh Actual,Glycol Pump Skid DayStart,Glycol Pump Skid MonthStart,Glycol Pump Skid YearStart</t>
+  </si>
+  <si>
+    <t>Glycol kWh Counter</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh Counter</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh Actual `%fanpanelnum`,Fan Panel kWh DayStart `%fanpanelnum`,Fan Panel kWh MonthStart `%fanpanelnum`,Fan Panel kWh YearStart `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh DayStart `%fanpanelnum`,Fan Panel kWh MonthStart `%fanpanelnum`,Fan Panel kWh YearStart `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Store Outside Temp,Cond kW Avg Demand `%rackname`,kW Avg Demand `%rackname`,Fan Panel kW Avg Demand `%fanpanelnum`,Glycol Pump Skid kW Actual</t>
+  </si>
+  <si>
+    <t>Performance kW Sum Predicted `%rackname`,Fan Panel kW Predicted `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Year `%rackname`,Fan Panel kWh YearCount `%fanpanelnum`,Glycol Pump Skid YearCount</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Month `%rackname`,Fan Panel kWh MonthCount `%fanpanelnum`,Glycol Pump Skid MonthCount</t>
+  </si>
+  <si>
+    <t>Op kWh Counter Current Day `%rackname`,Fan Panel kWh DayCount `%fanpanelnum`,Glycol Pump Skid DayCount</t>
+  </si>
+  <si>
+    <t>Cond kW Predicted `%rackname`,kW Predicted `%rackname`,Fan Panel kW Predicted `%fanpanelnum`,Glycol Pump Skid kW Predicted</t>
+  </si>
+  <si>
+    <t>Store Outside Temp,Cond kW Avg Demand `%rackname`,kW Avg Demand `%rackname`,Fan Panel kW Avg Demand `%fanpanelnum`,Glycol Pump Skid kW Avg Demand</t>
+  </si>
+  <si>
+    <t>Avg SEI</t>
+  </si>
+  <si>
+    <t>Avg COP</t>
+  </si>
+  <si>
+    <t>kWh to Dollars</t>
   </si>
 </sst>
 </file>
@@ -953,11 +989,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,16 +1039,16 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -1029,13 +1065,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -1055,7 +1091,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1081,13 +1117,13 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
@@ -1099,7 +1135,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1107,10 +1143,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>23</v>
@@ -1125,24 +1161,24 @@
         <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>31</v>
+        <v>202</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
@@ -1154,21 +1190,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>25</v>
@@ -1182,19 +1218,19 @@
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
@@ -1203,25 +1239,25 @@
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1229,24 +1265,24 @@
         <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -1260,152 +1296,152 @@
     </row>
     <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="B15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="F15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>8</v>
@@ -1416,22 +1452,22 @@
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>8</v>
@@ -1440,24 +1476,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>8</v>
@@ -1468,22 +1504,22 @@
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>8</v>
@@ -1494,22 +1530,22 @@
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>8</v>
@@ -1520,202 +1556,202 @@
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="E24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="F29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1726,21 +1762,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>98</v>
+        <v>198</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>7</v>
@@ -1754,19 +1790,19 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>7</v>
@@ -1780,19 +1816,19 @@
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>7</v>
@@ -1806,19 +1842,19 @@
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>7</v>
@@ -1832,71 +1868,71 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="B35" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="B36" s="2" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>56</v>
+        <v>200</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>7</v>
@@ -1908,21 +1944,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>75</v>
+        <v>199</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>7</v>
@@ -1936,19 +1972,19 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>7</v>
@@ -1962,22 +1998,22 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>8</v>
@@ -1988,22 +2024,22 @@
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>8</v>
@@ -2014,22 +2050,22 @@
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>8</v>
@@ -2038,55 +2074,107 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H43" s="1" t="s">
+      <c r="F45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Task fix to accommodate a different type of task
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="206">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -424,9 +424,6 @@
     <t>StoreCosts All Racks</t>
   </si>
   <si>
-    <t>Cond Fan Status `%rackname` `%sgname` `%compname`</t>
-  </si>
-  <si>
     <t>SEI_ALL_VALUES `%rackname`</t>
   </si>
   <si>
@@ -523,9 +520,6 @@
     <t>Cond Outlet Air Temperature `%rackname`,Cond Inlet Air Temperature `%rackname`</t>
   </si>
   <si>
-    <t>Cond Downleg Temperature `%rackname`,Cond Inlet Air Temperature `%rackname`</t>
-  </si>
-  <si>
     <t>Cond Ambient Subcooling `%rackname`</t>
   </si>
   <si>
@@ -592,9 +586,6 @@
     <t>Glycol Pump Skid kWh DayCount,Glycol Pump Skid kWh MonthCount,Glycol Pump Skid kWh YearCount</t>
   </si>
   <si>
-    <t>Glycol Pump Skid kWh Actual,Glycol Pump Skid DayStart,Glycol Pump Skid MonthStart,Glycol Pump Skid YearStart</t>
-  </si>
-  <si>
     <t>Glycol kWh Counter</t>
   </si>
   <si>
@@ -604,9 +595,6 @@
     <t>Fan Panel kWh Actual `%fanpanelnum`,Fan Panel kWh DayStart `%fanpanelnum`,Fan Panel kWh MonthStart `%fanpanelnum`,Fan Panel kWh YearStart `%fanpanelnum`</t>
   </si>
   <si>
-    <t>Fan Panel kWh DayStart `%fanpanelnum`,Fan Panel kWh MonthStart `%fanpanelnum`,Fan Panel kWh YearStart `%fanpanelnum`</t>
-  </si>
-  <si>
     <t>Store Outside Temp,Cond kW Avg Demand `%rackname`,kW Avg Demand `%rackname`,Fan Panel kW Avg Demand `%fanpanelnum`,Glycol Pump Skid kW Actual</t>
   </si>
   <si>
@@ -635,6 +623,15 @@
   </si>
   <si>
     <t>kWh to Dollars</t>
+  </si>
+  <si>
+    <t>Cond Downleg Temp `%rackname`,Cond Inlet Air Temperature `%rackname`</t>
+  </si>
+  <si>
+    <t>Glycol Pump Skid kWh Actual,Glycol Pump Skid kWh DayStart,Glycol Pump Skid kWh MonthStart,Glycol Pump Skid kWh YearStart</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh DayCount `%fanpanelnum`,Fan Panel kWh MonthCount `%fanpanelnum`,Fan Panel kWh YearCount `%fanpanelnum`</t>
   </si>
 </sst>
 </file>
@@ -992,20 +989,19 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="38.140625" style="4" customWidth="1"/>
     <col min="6" max="7" width="38.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1034,21 +1030,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>187</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -1065,13 +1061,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
@@ -1086,21 +1082,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -1109,24 +1105,24 @@
         <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>168</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -1135,287 +1131,287 @@
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>129</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>8</v>
@@ -1424,24 +1420,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>8</v>
@@ -1452,126 +1448,126 @@
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>8</v>
@@ -1582,22 +1578,22 @@
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>8</v>
@@ -1606,47 +1602,47 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>60</v>
@@ -1660,19 +1656,19 @@
     </row>
     <row r="26" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>184</v>
+        <v>67</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>69</v>
@@ -1686,19 +1682,19 @@
     </row>
     <row r="27" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>70</v>
@@ -1710,21 +1706,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>7</v>
@@ -1736,47 +1732,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>198</v>
+        <v>92</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>7</v>
@@ -1790,19 +1786,19 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>7</v>
@@ -1811,24 +1807,24 @@
         <v>8</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>7</v>
@@ -1840,21 +1836,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>7</v>
@@ -1866,9 +1862,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>144</v>
@@ -1877,10 +1873,10 @@
         <v>87</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>7</v>
@@ -1894,7 +1890,7 @@
     </row>
     <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>145</v>
@@ -1903,10 +1899,10 @@
         <v>87</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>7</v>
@@ -1920,7 +1916,7 @@
     </row>
     <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>146</v>
@@ -1929,10 +1925,10 @@
         <v>87</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>7</v>
@@ -1944,21 +1940,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>199</v>
+        <v>96</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>7</v>
@@ -1972,19 +1968,19 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>7</v>
@@ -1998,19 +1994,19 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>7</v>
@@ -2024,7 +2020,7 @@
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>149</v>
@@ -2033,10 +2029,10 @@
         <v>87</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>7</v>
@@ -2050,22 +2046,22 @@
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>8</v>
@@ -2076,22 +2072,22 @@
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>8</v>
@@ -2102,19 +2098,19 @@
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>110</v>
@@ -2126,24 +2122,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>8</v>
@@ -2152,24 +2148,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>8</v>
@@ -2179,6 +2175,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:H45">
+    <sortCondition ref="B2:B45"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added get stations and ios from DB rather than using excels
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -499,9 +499,6 @@
     <t>Rack SEI `%rackname`</t>
   </si>
   <si>
-    <t>COP `%rackname`,Rack SEI `%rackname`,Cond Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
-  </si>
-  <si>
     <t>Finds the difference between the cond variables</t>
   </si>
   <si>
@@ -632,6 +629,9 @@
   </si>
   <si>
     <t>Fan Panel kWh DayCount `%fanpanelnum`,Fan Panel kWh MonthCount `%fanpanelnum`,Fan Panel kWh YearCount `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>COP `%rackname`,Rack SEI `%rackname`,Cond Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`,Suction Saturation `%rackname` `%sgname`</t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1035,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1061,7 +1061,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -1110,19 +1110,19 @@
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -1139,16 +1139,16 @@
         <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
@@ -1162,19 +1162,19 @@
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
@@ -1223,10 +1223,10 @@
         <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
@@ -1249,7 +1249,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>30</v>
@@ -1266,19 +1266,19 @@
     </row>
     <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -1344,19 +1344,19 @@
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>7</v>
@@ -1373,16 +1373,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -1503,13 +1503,13 @@
         <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>41</v>
@@ -1529,7 +1529,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>48</v>
@@ -1555,7 +1555,7 @@
         <v>86</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>85</v>
@@ -1581,7 +1581,7 @@
         <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>85</v>
@@ -1590,7 +1590,7 @@
         <v>84</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>69</v>
@@ -1607,7 +1607,7 @@
         <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>85</v>
@@ -1616,7 +1616,7 @@
         <v>84</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>70</v>
@@ -1633,7 +1633,7 @@
         <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>59</v>
@@ -1659,7 +1659,7 @@
         <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>59</v>
@@ -1685,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>59</v>
@@ -1717,10 +1717,10 @@
         <v>52</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>7</v>
@@ -1821,7 +1821,7 @@
         <v>87</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>91</v>
@@ -1847,7 +1847,7 @@
         <v>87</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>117</v>
@@ -1873,7 +1873,7 @@
         <v>87</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>126</v>
@@ -1899,7 +1899,7 @@
         <v>87</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>127</v>
@@ -1925,7 +1925,7 @@
         <v>87</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Fan panel reset kWh tasks, fixed task imports to delete
</commit_message>
<xml_diff>
--- a/PanelCreator/src/Creator/textFiles/tasks.xlsx
+++ b/PanelCreator/src/Creator/textFiles/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="8805" windowHeight="6555"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="8805" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="taskSheet" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="215">
   <si>
     <t>task_manager_name</t>
   </si>
@@ -632,6 +632,33 @@
   </si>
   <si>
     <t>COP `%rackname`,Rack SEI `%rackname`,Cond Total Subcooling `%rackname`,Suction Superheat `%rackname` `%sgname`</t>
+  </si>
+  <si>
+    <t>Reset the Fan panels kWh counter at 12:01am</t>
+  </si>
+  <si>
+    <t>Reset the fan panels kWh counter at 12:01am</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh Actual `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh YearStart `%fanpanelnum`,Fan Panel kWh YearCount `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh MonthStart `%fanpanelnum`,Fan Panel kWh MonthCount `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Fan Panel kWh DayStart `%fanpanelnum`,Fan Panel kWh DayCount `%fanpanelnum`</t>
+  </si>
+  <si>
+    <t>Reset Fan Panels Day</t>
+  </si>
+  <si>
+    <t>Reset Fan Panels Month</t>
+  </si>
+  <si>
+    <t>Reset Fan Panels Year</t>
   </si>
 </sst>
 </file>
@@ -986,11 +1013,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,21 +1577,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>83</v>
+        <v>211</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>60</v>
@@ -1578,19 +1605,19 @@
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>69</v>
@@ -1602,21 +1629,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>70</v>
@@ -1628,21 +1655,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>60</v>
@@ -1654,21 +1681,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>67</v>
+        <v>181</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>69</v>
@@ -1680,21 +1707,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>70</v>
@@ -1706,151 +1733,151 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="F31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="F32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>7</v>
@@ -1862,21 +1889,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>196</v>
+        <v>89</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>7</v>
@@ -1885,24 +1912,24 @@
         <v>8</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>7</v>
@@ -1914,21 +1941,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>7</v>
@@ -1940,21 +1967,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>7</v>
@@ -1966,21 +1993,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>97</v>
+        <v>195</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>7</v>
@@ -1992,21 +2019,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>7</v>
@@ -2020,19 +2047,19 @@
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>7</v>
@@ -2046,19 +2073,19 @@
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>7</v>
@@ -2072,19 +2099,19 @@
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>7</v>
@@ -2098,22 +2125,22 @@
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>8</v>
@@ -2124,22 +2151,22 @@
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>8</v>
@@ -2150,27 +2177,105 @@
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="1" t="s">
+      <c r="G48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>